<commit_message>
TIC-8 Ticketplan FTP documentation (#196)
</commit_message>
<xml_diff>
--- a/source/products/ticketplan/files/ticketplan_import.xlsx
+++ b/source/products/ticketplan/files/ticketplan_import.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janisdavidsons/Documents/ticketplan-svc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86F7CC76-2FB6-EB4E-919C-9FF0234C3048}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7151196-E46D-8746-B162-C1B0C7A37A99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="56">
   <si>
     <t>idempotency_key</t>
   </si>
@@ -195,6 +195,12 @@
   </si>
   <si>
     <t>john.smith@com</t>
+  </si>
+  <si>
+    <t>policy.data.order_currency</t>
+  </si>
+  <si>
+    <t>euro</t>
   </si>
 </sst>
 </file>
@@ -551,10 +557,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AE3"/>
+  <dimension ref="A1:AF3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="AA1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="AD15" sqref="AD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -589,9 +595,10 @@
     <col min="29" max="29" width="30.6640625" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="32.83203125" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="25.1640625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -685,8 +692,11 @@
       <c r="AE1" t="s">
         <v>27</v>
       </c>
+      <c r="AF1" t="s">
+        <v>54</v>
+      </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>48</v>
       </c>
@@ -780,8 +790,11 @@
       <c r="AE2">
         <v>2</v>
       </c>
+      <c r="AF2" t="s">
+        <v>55</v>
+      </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>49</v>
       </c>
@@ -874,6 +887,9 @@
       </c>
       <c r="AE3">
         <v>2</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ticketplan FTP doc adjustment
</commit_message>
<xml_diff>
--- a/source/products/ticketplan/files/ticketplan_import.xlsx
+++ b/source/products/ticketplan/files/ticketplan_import.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janisdavidsons/Documents/ticketplan-svc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janisdavidsons/src/kasko/apps/docs/source/products/ticketplan/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7151196-E46D-8746-B162-C1B0C7A37A99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{481AECB2-9F4A-5340-B8FD-494DBF457E41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="9820" windowWidth="51200" windowHeight="16760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="59">
   <si>
     <t>idempotency_key</t>
   </si>
@@ -74,9 +74,6 @@
     <t>policy.data.event_name</t>
   </si>
   <si>
-    <t>policy.data.event_date</t>
-  </si>
-  <si>
     <t>policy.data.venue_name</t>
   </si>
   <si>
@@ -201,6 +198,18 @@
   </si>
   <si>
     <t>euro</t>
+  </si>
+  <si>
+    <t>policy.data.event_end_date</t>
+  </si>
+  <si>
+    <t>policy.data.event_start_date</t>
+  </si>
+  <si>
+    <t>integration_id</t>
+  </si>
+  <si>
+    <t>in_41c2f22d51612f04ee2c48eca3dc0</t>
   </si>
 </sst>
 </file>
@@ -557,346 +566,366 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AF3"/>
+  <dimension ref="A1:AH3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AA1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="AD15" sqref="AD15"/>
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="34.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="30.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.6640625" customWidth="1"/>
-    <col min="10" max="10" width="13" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="22.1640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.5" customWidth="1"/>
-    <col min="16" max="16" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="19.83203125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="22.1640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="21.83203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="24" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="30" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="22.83203125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="21.1640625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="25.5" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="32.83203125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="25.1640625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="21.6640625" customWidth="1"/>
+    <col min="2" max="2" width="34.5" customWidth="1"/>
+    <col min="3" max="3" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="30.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.6640625" customWidth="1"/>
+    <col min="11" max="11" width="13" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.5" customWidth="1"/>
+    <col min="17" max="17" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="31.6640625" customWidth="1"/>
+    <col min="19" max="19" width="29.6640625" customWidth="1"/>
+    <col min="20" max="20" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="24" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="30" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="32.83203125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="25.1640625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="G1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M1" t="s">
-        <v>10</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R1" t="s">
+        <v>56</v>
+      </c>
+      <c r="S1" t="s">
+        <v>55</v>
+      </c>
+      <c r="T1" t="s">
+        <v>13</v>
+      </c>
+      <c r="U1" t="s">
+        <v>14</v>
+      </c>
+      <c r="V1" t="s">
+        <v>15</v>
+      </c>
+      <c r="W1" t="s">
+        <v>16</v>
+      </c>
+      <c r="X1" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="P1" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>13</v>
-      </c>
-      <c r="R1" t="s">
-        <v>14</v>
-      </c>
-      <c r="S1" t="s">
-        <v>15</v>
-      </c>
-      <c r="T1" t="s">
-        <v>16</v>
-      </c>
-      <c r="U1" t="s">
-        <v>17</v>
-      </c>
-      <c r="V1" t="s">
-        <v>18</v>
-      </c>
-      <c r="W1" t="s">
-        <v>19</v>
-      </c>
-      <c r="X1" t="s">
-        <v>20</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>21</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>22</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>23</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AE1" t="s">
+      <c r="B2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" t="s">
         <v>27</v>
       </c>
-      <c r="AF1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2">
+      <c r="D2">
         <v>1</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>0</v>
-      </c>
-      <c r="E2">
-        <v>3000</v>
       </c>
       <c r="F2">
         <v>3000</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2">
+        <v>3000</v>
+      </c>
+      <c r="H2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" t="s">
         <v>29</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="K2" t="s">
         <v>30</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="J2" t="s">
+      <c r="L2" t="s">
         <v>31</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
+        <v>31</v>
+      </c>
+      <c r="N2">
+        <v>2</v>
+      </c>
+      <c r="O2">
+        <v>5597</v>
+      </c>
+      <c r="P2">
+        <v>100000</v>
+      </c>
+      <c r="Q2" t="s">
         <v>32</v>
       </c>
-      <c r="L2" t="s">
-        <v>32</v>
-      </c>
-      <c r="M2">
+      <c r="R2" t="s">
+        <v>33</v>
+      </c>
+      <c r="S2" t="s">
+        <v>33</v>
+      </c>
+      <c r="T2" t="s">
+        <v>34</v>
+      </c>
+      <c r="U2" t="s">
+        <v>35</v>
+      </c>
+      <c r="V2" t="s">
+        <v>36</v>
+      </c>
+      <c r="W2" t="s">
+        <v>37</v>
+      </c>
+      <c r="X2" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA2">
+        <v>123</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AD2">
+        <v>44444</v>
+      </c>
+      <c r="AE2">
+        <v>55555</v>
+      </c>
+      <c r="AF2">
+        <v>55555</v>
+      </c>
+      <c r="AG2">
         <v>2</v>
       </c>
-      <c r="N2">
-        <v>5597</v>
-      </c>
-      <c r="O2">
-        <v>100000</v>
-      </c>
-      <c r="P2" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>34</v>
-      </c>
-      <c r="R2" t="s">
-        <v>35</v>
-      </c>
-      <c r="S2" t="s">
-        <v>36</v>
-      </c>
-      <c r="T2" t="s">
-        <v>37</v>
-      </c>
-      <c r="U2" t="s">
-        <v>38</v>
-      </c>
-      <c r="V2" t="s">
-        <v>39</v>
-      </c>
-      <c r="W2" t="s">
-        <v>29</v>
-      </c>
-      <c r="X2" t="s">
-        <v>30</v>
-      </c>
-      <c r="Y2">
-        <v>123</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>40</v>
-      </c>
-      <c r="AA2" t="s">
+      <c r="AH2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" t="s">
         <v>41</v>
       </c>
-      <c r="AB2">
-        <v>44444</v>
-      </c>
-      <c r="AC2">
-        <v>55555</v>
-      </c>
-      <c r="AD2">
-        <v>55555</v>
-      </c>
-      <c r="AE2">
-        <v>2</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C3">
+      <c r="D3">
         <v>1</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>0</v>
-      </c>
-      <c r="E3">
-        <v>3000</v>
       </c>
       <c r="F3">
         <v>3000</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3">
+        <v>3000</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="J3" t="s">
-        <v>31</v>
+      <c r="J3" s="2" t="s">
+        <v>52</v>
       </c>
       <c r="K3" t="s">
+        <v>30</v>
+      </c>
+      <c r="L3" t="s">
+        <v>42</v>
+      </c>
+      <c r="M3" t="s">
+        <v>42</v>
+      </c>
+      <c r="N3">
+        <v>2</v>
+      </c>
+      <c r="O3">
+        <v>8685</v>
+      </c>
+      <c r="P3">
+        <v>100000</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>32</v>
+      </c>
+      <c r="R3" t="s">
+        <v>33</v>
+      </c>
+      <c r="S3" t="s">
         <v>43</v>
       </c>
-      <c r="L3" t="s">
-        <v>43</v>
-      </c>
-      <c r="M3">
+      <c r="T3" t="s">
+        <v>34</v>
+      </c>
+      <c r="U3" t="s">
+        <v>35</v>
+      </c>
+      <c r="V3" t="s">
+        <v>36</v>
+      </c>
+      <c r="W3" t="s">
+        <v>37</v>
+      </c>
+      <c r="X3" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA3">
+        <v>123</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AD3">
+        <v>44444</v>
+      </c>
+      <c r="AE3">
+        <v>55555</v>
+      </c>
+      <c r="AF3">
+        <v>55555</v>
+      </c>
+      <c r="AG3">
         <v>2</v>
       </c>
-      <c r="N3">
-        <v>8685</v>
-      </c>
-      <c r="O3">
-        <v>100000</v>
-      </c>
-      <c r="P3" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>44</v>
-      </c>
-      <c r="R3" t="s">
-        <v>35</v>
-      </c>
-      <c r="S3" t="s">
-        <v>36</v>
-      </c>
-      <c r="T3" t="s">
-        <v>37</v>
-      </c>
-      <c r="U3" t="s">
-        <v>38</v>
-      </c>
-      <c r="V3" t="s">
-        <v>39</v>
-      </c>
-      <c r="W3" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="X3" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y3">
-        <v>123</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>41</v>
-      </c>
-      <c r="AB3">
-        <v>44444</v>
-      </c>
-      <c r="AC3">
-        <v>55555</v>
-      </c>
-      <c r="AD3">
-        <v>55555</v>
-      </c>
-      <c r="AE3">
-        <v>2</v>
-      </c>
-      <c r="AF3" t="s">
-        <v>55</v>
+      <c r="AH3" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1" xr:uid="{ACAB6086-6C11-134D-B740-3EB197CC1375}"/>
-    <hyperlink ref="I3" r:id="rId2" xr:uid="{71DB3B38-1EF4-5340-9703-89BAF2B43959}"/>
+    <hyperlink ref="J2" r:id="rId1" xr:uid="{ACAB6086-6C11-134D-B740-3EB197CC1375}"/>
+    <hyperlink ref="J3" r:id="rId2" xr:uid="{71DB3B38-1EF4-5340-9703-89BAF2B43959}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>